<commit_message>
atualizações e telas de pgto
</commit_message>
<xml_diff>
--- a/Produtos para Banco.xlsx
+++ b/Produtos para Banco.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Organize\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Projeto_Final_e-commerce\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB73593A-44A4-4B32-8B43-9A8C679C3845}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A951017-F0C9-4DA2-94B0-6E6B676614A0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19560" windowHeight="8130" xr2:uid="{B17280E4-21C7-4FAE-8449-26292023E485}"/>
   </bookViews>
@@ -1166,7 +1166,7 @@
     <col min="3" max="3" width="21.42578125" style="12" customWidth="1"/>
     <col min="4" max="4" width="20.5703125" style="1" customWidth="1"/>
     <col min="5" max="6" width="9.28515625" style="13" customWidth="1"/>
-    <col min="7" max="7" width="68" style="12" customWidth="1"/>
+    <col min="7" max="7" width="72.7109375" style="12" customWidth="1"/>
     <col min="8" max="8" width="15.85546875" style="1" customWidth="1"/>
     <col min="9" max="9" width="55.42578125" style="13" customWidth="1"/>
     <col min="10" max="10" width="16" style="18" customWidth="1"/>
@@ -1191,7 +1191,7 @@
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" s="24" t="str">
-        <f t="shared" ref="B4:B28" si="0">"("&amp;B44&amp;",'"&amp;C44&amp;"', '"&amp;D44&amp;"', '"&amp;E44&amp;"', '"&amp;F44&amp;"', '"&amp;G44&amp;"', "&amp;H44&amp;", '"&amp;I44&amp;"', "&amp;J44&amp;", '"&amp;K44&amp;"'),"</f>
+        <f t="shared" ref="B4:B26" si="0">"("&amp;B44&amp;",'"&amp;C44&amp;"', '"&amp;D44&amp;"', '"&amp;E44&amp;"', '"&amp;F44&amp;"', '"&amp;G44&amp;"', "&amp;H44&amp;", '"&amp;I44&amp;"', "&amp;J44&amp;", '"&amp;K44&amp;"'),"</f>
         <v>(2,'AAS - Salicetil 100 mg Infantil com 200 Comprimidos', 'Brasterápica', 'n/d', '1002', 'img/produtos/Medicamentos/Salicetil_Analgesico_Antitermico.jpg', 12.09, 'Informações do Produto
 Indicações: Para o alívio sintomático de dores de intensidade leve a moderada, como dor de cabeça, dor de dente, dor de garganta, dor menstrual, dor muscular, dor nas articulações, dor nas costas, dor da artrite; alívio sintomático da dor e da febre nos resfriados ou gripes.
 Contraindicações: Hipersensibilidade (alergia) ao ácido acetilsalicílico ou a qualquer outro componente do medicamento. Histórico de crise de asma induzida pela administração de salicilatos ou outras substâncias de ação semelhante, especialmente antiinflamatórios não esteroidais; úlceras do estômago ou do intestino (úlceras gastrintestinais agudas); tendência para sangramentos (diátese hemorrágica); alteração grave da função dos rins (insuficiência renal grave); alteração grave da função do fígado (insuficiência hepática grave); alteração grave da função do coração (insuficiência cardíaca grave); tratamento com metotrexato em doses iguais ou superiores a 15 mg por semana; último trimestre de gravidez. Este medicamento não deve ser utilizado por mulheres grávidas sem orientação médica.', 1, 'bulas/bula.pdf'),</v>
@@ -1920,7 +1920,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="55" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" s="1">
         <v>13</v>
       </c>

</xml_diff>